<commit_message>
updated metadata. added source data, added modified notebook
</commit_message>
<xml_diff>
--- a/Enforcement Tracker info/IE_metadata.xlsx
+++ b/Enforcement Tracker info/IE_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annguyen\Desktop\School\IBS-Capstone-Project\Enforcement Tracker info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annguyen\Desktop\School\IBS-Capstone-Project-1\IBS-Capstone-Project\Enforcement Tracker info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECBF7BD1-1E38-4588-800B-19D30DE4EFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D13A4F28-9199-44A8-ABA3-D3A5A47323F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{208EFAE7-3608-45F7-8BE2-D99924AF8437}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{138079E2-6100-4424-B6D5-212E60ABDD98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,35 +36,122 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="195">
+  <si>
+    <t>ETid-2780</t>
+  </si>
+  <si>
+    <t>IRELAND</t>
+  </si>
+  <si>
+    <t>Data Protection Authority of Ireland</t>
+  </si>
+  <si>
+    <t>Maynooth University</t>
+  </si>
+  <si>
+    <t>Public Sector and Education</t>
+  </si>
+  <si>
+    <t>Art. 5 (1) f) GDPR, Art. 32 (1) GDPR, Art. 33 (1) GDPR</t>
+  </si>
+  <si>
+    <t>Insufficient technical and organisational measures to ensure information security</t>
+  </si>
+  <si>
+    <t>The Irish DPA has imposed a fine of EUR 40,000 on Maynooth University. The controller failed to implement adequate technical and organisational measures, resulting in an unauthorised third party gaining access to multiple employees' email accounts, which the third party then used for fraudulent purposes.</t>
+  </si>
+  <si>
+    <t>link link</t>
+  </si>
+  <si>
+    <t>https://www.enforcementtracker.com/ETid-2780 (Copy: ) | Short URL: https://etid.link/ETid-2780</t>
+  </si>
+  <si>
+    <t>ETid-2779</t>
+  </si>
+  <si>
+    <t>Sligo County Council</t>
+  </si>
+  <si>
+    <t>Art. 5 (1) a), c), e), f) GDPR, Art. 13 (1), (3) GDPR, Art. 24 (1) GDPR, Art. 25 GDPR, Art. 30 GDPR, Art. 32 (1) GDPR</t>
+  </si>
+  <si>
+    <t>Non-compliance with general data processing principles</t>
+  </si>
+  <si>
+    <t>The Irish DPA has imposed a fine of EUR 29,500 on the Sligo County Council. The controller used video surveillance but failed to ensure compliance with the GDPR. They failed to provide adequate information to data subjects, failed to implement sufficient technical and organisational measures to ensure GDPR compliance, failed to ensure adequate data security and stored the recorded data for longer than necessary.</t>
+  </si>
+  <si>
+    <t>https://www.enforcementtracker.com/ETid-2779 (Copy: ) | Short URL: https://etid.link/ETid-2779</t>
+  </si>
+  <si>
+    <t>ETid-2684</t>
+  </si>
+  <si>
+    <t>City of Dublin Education and Training Board</t>
+  </si>
+  <si>
+    <t>Art. 5 (1) f) GDPR, Art. 32 (1), (2) GDPR, Art. 33 (1) GDPR, Art. 34 (1), (4) GDPR</t>
+  </si>
+  <si>
+    <t>The Irish DPA has imposed a fine of EUR 125,000 on the City of Dublin Education and Training Board. The controller suffered a data breach due to insufficient technical and organisational measures, concerning around 13,000 data subjects. The controller also failed to inform the DPC and the data subjects without undue delay.</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>https://www.enforcementtracker.com/ETid-2684 (Copy: ) | Short URL: https://etid.link/ETid-2684</t>
+  </si>
+  <si>
+    <t>ETid-2657</t>
+  </si>
+  <si>
+    <t>Departement of Social Security</t>
+  </si>
+  <si>
+    <t>Art. 5 (1) a), e) GDPR, Art. 6 (1) GDPR, Art. 9 (1) GDPR, Art. 13 (1) c) GDPR, Art. 13 (2) a) GDPR, Art. 35 (VII) b), c) GDPR</t>
+  </si>
+  <si>
+    <t>Insufficient legal basis for data processing</t>
+  </si>
+  <si>
+    <t>The Irish DPA imposed a fine of EUR 550,000 on the Departement of Social Security. The controller uses the so called SAFE 2 registration process for anyone applying for a Public Services Card. The SAFE 2 registration, which is mandatory, processes biometric data without a sufficient legal basis. The controller also failed to adequately inform data subjects in regards to the processing and to conduct a data protection impact assessment.</t>
+  </si>
+  <si>
+    <t>https://www.enforcementtracker.com/ETid-2657 (Copy: ) | Short URL: https://etid.link/ETid-2657</t>
+  </si>
+  <si>
+    <t>ETid-2584</t>
+  </si>
+  <si>
+    <t>TikTok Technology Limited</t>
+  </si>
+  <si>
+    <t>Media, Telecoms and Broadcasting</t>
+  </si>
+  <si>
+    <t>Art. 13 (1) f) GDPR, Art. 46 (1) GDPR</t>
+  </si>
+  <si>
+    <t>The Irish DPA (DPC) has fined TikTok EUR 530 million. In its decision, the DPC found, that TikTok infringed Art. 13 (1) f) GDPR and Art. 46 (1) GDPR due to the unlawful transfer and storage of personal data from users in the EEA on Chinese servers. TikTok was unable to verify, guarantee and demonstrate that the supplementary measures and the Standard Contractual Clauses were effective to guarantee that the data afforded a level of protection, which is equivalent of the level of protection guaranteed in the EU. TikTok also failed to inform the data subjects, that their personal data is transferred to a third country. The fine consists of a fine of EUR 45 million for the failure to inform the data subjects and a fine of EUR 485 million for the infringement of Art. 46 (1) GDPR. The DPC also ordered TikTok to bring their processes into compliance with the GDPR within 6 months after the period allowed for an appeal against the DPCs final decision.</t>
+  </si>
+  <si>
+    <t>https://www.enforcementtracker.com/ETid-2584 (Copy: ) | Short URL: https://etid.link/ETid-2584</t>
+  </si>
   <si>
     <t>ETid-2484</t>
   </si>
   <si>
-    <t>IRELAND</t>
-  </si>
-  <si>
-    <t>Data Protection Authority of Ireland</t>
-  </si>
-  <si>
     <t>Meta Platforms Ireland Limited</t>
   </si>
   <si>
-    <t>Media, Telecoms and Broadcasting</t>
-  </si>
-  <si>
     <t>Art. 33 (3), (5) GDPR, Art. 25 (1), (2) GDPR</t>
   </si>
   <si>
-    <t>Insufficient technical and organisational measures to ensure information security</t>
-  </si>
-  <si>
     <t>The Irish Data Protection Commission (DPC) has fined Meta Platforms Ireland Limited EUR 251 million. The fine was imposed for data protection violations related to a data breach that occurred in 2018 and affected 29 million Facebook accounts worldwide, including 3 million in the EU/EEA. Compromised data included names, email addresses, phone numbers, and children's data. The breach resulted from the exploitation of user tokens on the platform by unauthorized third parties. The DPC found that Meta had violated Art. 33 GDPR (EUR 11 million), as information was missing from the data breach notification, for example. The DPC also found violations of Art. 25 GDPR (EUR 240 million), concluding that Meta had failed to ensure that data protection principles were protected in the design of processing systems and had failed in its obligations as a controller to ensure that, by default, only personal data that are necessary for specific purposes are processed.</t>
   </si>
   <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>https://www.enforcementtracker.com/ETid-2484 (Copy: ) | Short URL: https://etid.link/ETid-2484</t>
   </si>
   <si>
@@ -75,9 +162,6 @@
   </si>
   <si>
     <t>Art. 5 (1) a) GDPR, Art. 6 (1) a), e), f) GDPR, Art. 13 (1) c) GDPR, Art. 14 (1) c) GDPR</t>
-  </si>
-  <si>
-    <t>Insufficient legal basis for data processing</t>
   </si>
   <si>
     <t>The Irish DPA (DPC) has fined LinkedIn EUR 310 million. This decision is related to an investigation following a complaint in 2018 from the French NGO 'La Quadrature Du Net'. In July 2024, the DPC issued a draft decision under the GDPR cooperation mechanism under Art. 60 GDPR, to which no objections were raised.
@@ -112,9 +196,6 @@
     <t>Art. 5 (1) c), 5 (1) f) GDPR, Art. 12 (1) GDPR, Art. 13 (1) e) GDPR, Art. 24 (1) GDPR, Art. 25 (1), (2) GDPR</t>
   </si>
   <si>
-    <t>Non-compliance with general data processing principles</t>
-  </si>
-  <si>
     <t>The Irish DPA (DPC), has imposed a fine of EUR 345 million on TikTok Limited. The DPC conducted an investigation primarily focused on the processing of personal data between July 31, 2020, and December 31, 2020. During their investigation, the DPC found that the profiles of child users were set to public access by default. As a result, the DPC concluded that TikTok had failed to implement appropriate technical and organizational measures to ensure that only necessary personal data was being processed.
 Furthermore, the DPC noted that the 'Family Pairing' feature, which allowed non-child users to link their accounts with those of child users, posed a security risk to the personal data of children.
 Additionally, TikTok failed to provide child users with information about the categories of recipients of their personal data and clear, understandable information on the scope and implications of data processing.
@@ -155,9 +236,6 @@
 Following the investigation, the DPC submitted a draft decision to other concerned supervisory authorities pursuant to Art. 60 GDPR. In response, the DPC received objections from supervisory authorities, which led to a dispute resolution procedure before the European Data Protection Board (EDPB). In its decision, the EDPB asked the DPC to amend the proposed fine and adapt it to the seriousness of the data protection breach.
 The DPC also ordered to cease any future transfer of personal data to the U.S., as well as to cease storage, within six months, of data already transferred to the U.S.
 Meta has announced that it will appeal the ruling and seek a suspension of the orders in court.</t>
-  </si>
-  <si>
-    <t>link link</t>
   </si>
   <si>
     <t>https://www.enforcementtracker.com/ETid-1844 (Copy: ) | Short URL: https://etid.link/ETid-1844</t>
@@ -355,9 +433,6 @@
   </si>
   <si>
     <t>Limerick City and County Council</t>
-  </si>
-  <si>
-    <t>Public Sector and Education</t>
   </si>
   <si>
     <t>Art. 13 GDPR, Art. 12 GPDR, Art. 15 GDPR</t>
@@ -645,9 +720,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -987,68 +1063,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D490337-EEFD-4B43-BAF8-11BAFFB931BB}">
-  <dimension ref="B1:M31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE5B08C-03E7-4F8D-90FA-A98C1948C125}">
+  <dimension ref="B1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="84.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="66.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="79.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="103.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="86.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1059,10 +1135,10 @@
         <v>2</v>
       </c>
       <c r="E2" s="1">
-        <v>45643</v>
-      </c>
-      <c r="F2" s="5">
-        <v>251000000</v>
+        <v>45618</v>
+      </c>
+      <c r="F2" s="2">
+        <v>40000</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -1086,7 +1162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1097,10 +1173,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>45589</v>
-      </c>
-      <c r="F3" s="5">
-        <v>310000000</v>
+        <v>45609</v>
+      </c>
+      <c r="F3" s="2">
+        <v>29500</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -1114,7 +1190,7 @@
       <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
       <c r="L3" t="s">
@@ -1124,7 +1200,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1135,36 +1211,36 @@
         <v>2</v>
       </c>
       <c r="E4" s="1">
-        <v>45562</v>
-      </c>
-      <c r="F4" s="5">
-        <v>91000000</v>
+        <v>45831</v>
+      </c>
+      <c r="F4" s="2">
+        <v>125000</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>18</v>
+      <c r="K4" t="s">
+        <v>19</v>
       </c>
       <c r="L4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="M4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1173,244 +1249,244 @@
         <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>45170</v>
-      </c>
-      <c r="F5" s="5">
-        <v>345000000</v>
+        <v>45820</v>
+      </c>
+      <c r="F5" s="2">
+        <v>550000</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
       </c>
       <c r="L5" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="M5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45779</v>
+      </c>
+      <c r="F6" s="2">
+        <v>530000000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>45093</v>
-      </c>
-      <c r="F6" s="5">
-        <v>22500</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45643</v>
+      </c>
+      <c r="F7" s="2">
+        <v>251000000</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="L6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>45058</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1200000000</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>4</v>
-      </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>34</v>
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
       </c>
       <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45589</v>
+      </c>
+      <c r="F8" s="2">
+        <v>310000000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45562</v>
+      </c>
+      <c r="F9" s="2">
+        <v>91000000</v>
+      </c>
+      <c r="G9" t="s">
         <v>35</v>
       </c>
-      <c r="M7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1">
-        <v>44984</v>
-      </c>
-      <c r="F8" s="5">
-        <v>750000</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1">
-        <v>44925</v>
-      </c>
-      <c r="F9" s="5">
-        <v>15000</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
       <c r="H9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
         <v>45</v>
-      </c>
-      <c r="I9" t="s">
-        <v>46</v>
       </c>
       <c r="J9" t="s">
         <v>6</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" t="s">
         <v>47</v>
       </c>
-      <c r="L9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9" t="s">
+    </row>
+    <row r="10" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>45170</v>
+      </c>
+      <c r="F10" s="2">
+        <v>345000000</v>
+      </c>
+      <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="1">
-        <v>44949</v>
-      </c>
-      <c r="F10" s="5">
-        <v>460000</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" t="s">
         <v>50</v>
       </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
         <v>52</v>
       </c>
-      <c r="L10" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" t="s">
+    </row>
+    <row r="11" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>45093</v>
+      </c>
+      <c r="F11" s="2">
+        <v>22500</v>
+      </c>
+      <c r="G11" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1">
-        <v>44945</v>
-      </c>
-      <c r="F11" s="5">
-        <v>5500000</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>55</v>
-      </c>
-      <c r="H11" t="s">
-        <v>4</v>
       </c>
       <c r="I11" t="s">
         <v>56</v>
@@ -1418,17 +1494,17 @@
       <c r="J11" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="3" t="s">
         <v>57</v>
       </c>
       <c r="L11" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="M11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>59</v>
       </c>
@@ -1439,74 +1515,74 @@
         <v>2</v>
       </c>
       <c r="E12" s="1">
-        <v>44917</v>
-      </c>
-      <c r="F12" s="5">
-        <v>100000</v>
+        <v>45058</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1200000000</v>
       </c>
       <c r="G12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
         <v>60</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="I12" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" t="s">
         <v>62</v>
       </c>
-      <c r="L12" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" t="s">
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>44984</v>
+      </c>
+      <c r="F13" s="2">
+        <v>750000</v>
+      </c>
+      <c r="G13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="1">
-        <v>44930</v>
-      </c>
-      <c r="F13" s="5">
-        <v>390000000</v>
-      </c>
-      <c r="G13" t="s">
-        <v>3</v>
-      </c>
       <c r="H13" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="I13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>66</v>
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
+        <v>67</v>
       </c>
       <c r="L13" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="M13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1515,224 +1591,224 @@
         <v>2</v>
       </c>
       <c r="E14" s="1">
-        <v>44587</v>
-      </c>
-      <c r="F14" s="5">
-        <v>5000</v>
+        <v>44925</v>
+      </c>
+      <c r="F14" s="2">
+        <v>15000</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H14" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="I14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J14" t="s">
         <v>6</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>71</v>
+      <c r="K14" t="s">
+        <v>73</v>
       </c>
       <c r="L14" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>44949</v>
+      </c>
+      <c r="F15" s="2">
+        <v>460000</v>
+      </c>
+      <c r="G15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1">
+        <v>44945</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5500000</v>
+      </c>
+      <c r="G16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="L16" t="s">
         <v>8</v>
       </c>
-      <c r="M14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>44890</v>
-      </c>
-      <c r="F15" s="5">
-        <v>265000000</v>
-      </c>
-      <c r="G15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="M16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44917</v>
+      </c>
+      <c r="F17" s="2">
+        <v>100000</v>
+      </c>
+      <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44930</v>
+      </c>
+      <c r="F18" s="2">
+        <v>390000000</v>
+      </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="L18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>44587</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G19" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I19" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L15" t="s">
-        <v>35</v>
-      </c>
-      <c r="M15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1">
-        <v>44809</v>
-      </c>
-      <c r="F16" s="5">
-        <v>405000000</v>
-      </c>
-      <c r="G16" t="s">
-        <v>78</v>
-      </c>
-      <c r="H16" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" t="s">
-        <v>79</v>
-      </c>
-      <c r="J16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="L16" t="s">
-        <v>81</v>
-      </c>
-      <c r="M16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>44656</v>
-      </c>
-      <c r="F17" s="5">
-        <v>463000</v>
-      </c>
-      <c r="G17" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" t="s">
-        <v>35</v>
-      </c>
-      <c r="M17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1">
-        <v>44635</v>
-      </c>
-      <c r="F18" s="5">
-        <v>17000000</v>
-      </c>
-      <c r="G18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" t="s">
-        <v>89</v>
-      </c>
-      <c r="J18" t="s">
-        <v>6</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L18" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="1">
-        <v>44539</v>
-      </c>
-      <c r="F19" s="5">
-        <v>110000</v>
-      </c>
-      <c r="G19" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" t="s">
-        <v>94</v>
-      </c>
-      <c r="I19" t="s">
-        <v>95</v>
-      </c>
-      <c r="J19" t="s">
-        <v>96</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="3" t="s">
         <v>97</v>
       </c>
       <c r="L19" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="M19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>99</v>
       </c>
@@ -1743,72 +1819,72 @@
         <v>2</v>
       </c>
       <c r="E20" s="1">
-        <v>44532</v>
-      </c>
-      <c r="F20" s="5">
-        <v>60000</v>
+        <v>44890</v>
+      </c>
+      <c r="F20" s="2">
+        <v>265000000</v>
       </c>
       <c r="G20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" t="s">
+        <v>30</v>
+      </c>
+      <c r="I20" t="s">
         <v>100</v>
-      </c>
-      <c r="H20" t="s">
-        <v>94</v>
-      </c>
-      <c r="I20" t="s">
-        <v>101</v>
       </c>
       <c r="J20" t="s">
         <v>6</v>
       </c>
-      <c r="K20" s="2" t="s">
-        <v>102</v>
+      <c r="K20" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="L20" t="s">
         <v>8</v>
       </c>
       <c r="M20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1">
+        <v>44809</v>
+      </c>
+      <c r="F21" s="2">
+        <v>405000000</v>
+      </c>
+      <c r="G21" t="s">
         <v>104</v>
       </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="1">
-        <v>44428</v>
-      </c>
-      <c r="F21" s="5">
-        <v>1500</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" t="s">
         <v>105</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="I21" t="s">
-        <v>40</v>
-      </c>
-      <c r="J21" t="s">
-        <v>6</v>
-      </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" t="s">
         <v>107</v>
-      </c>
-      <c r="L21" t="s">
-        <v>35</v>
       </c>
       <c r="M21" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>109</v>
       </c>
@@ -1819,176 +1895,176 @@
         <v>2</v>
       </c>
       <c r="E22" s="1">
-        <v>44475</v>
-      </c>
-      <c r="F22" s="5" t="s">
+        <v>44656</v>
+      </c>
+      <c r="F22" s="2">
+        <v>463000</v>
+      </c>
+      <c r="G22" t="s">
         <v>110</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" t="s">
         <v>111</v>
       </c>
-      <c r="H22" t="s">
-        <v>4</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="J22" t="s">
-        <v>113</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="L22" t="s">
         <v>8</v>
       </c>
       <c r="M22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>44635</v>
+      </c>
+      <c r="F23" s="2">
+        <v>17000000</v>
+      </c>
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="J23" t="s">
+        <v>6</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="1">
-        <v>44446</v>
-      </c>
-      <c r="F23" s="5">
-        <v>1400</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="L23" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" t="s">
         <v>117</v>
       </c>
-      <c r="H23" t="s">
-        <v>4</v>
-      </c>
-      <c r="I23" t="s">
+    </row>
+    <row r="24" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>118</v>
       </c>
-      <c r="J23" t="s">
-        <v>96</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>44539</v>
+      </c>
+      <c r="F24" s="2">
+        <v>110000</v>
+      </c>
+      <c r="G24" t="s">
         <v>119</v>
-      </c>
-      <c r="L23" t="s">
-        <v>8</v>
-      </c>
-      <c r="M23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>44441</v>
-      </c>
-      <c r="F24" s="5">
-        <v>225000000</v>
-      </c>
-      <c r="G24" t="s">
-        <v>55</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
       </c>
       <c r="I24" t="s">
+        <v>120</v>
+      </c>
+      <c r="J24" t="s">
+        <v>121</v>
+      </c>
+      <c r="K24" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J24" t="s">
-        <v>113</v>
-      </c>
-      <c r="K24" s="2" t="s">
+      <c r="L24" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24" t="s">
         <v>123</v>
       </c>
-      <c r="L24" t="s">
-        <v>35</v>
-      </c>
-      <c r="M24" t="s">
+    </row>
+    <row r="25" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>44532</v>
+      </c>
+      <c r="F25" s="2">
+        <v>60000</v>
+      </c>
+      <c r="G25" t="s">
         <v>125</v>
       </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1">
-        <v>44278</v>
-      </c>
-      <c r="F25" s="5">
-        <v>90000</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" t="s">
         <v>126</v>
-      </c>
-      <c r="H25" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25" t="s">
-        <v>127</v>
       </c>
       <c r="J25" t="s">
         <v>6</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L25" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" t="s">
         <v>128</v>
       </c>
-      <c r="L25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M25" t="s">
+    </row>
+    <row r="26" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>44428</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1500</v>
+      </c>
+      <c r="G26" t="s">
         <v>130</v>
       </c>
-      <c r="C26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1">
-        <v>44055</v>
-      </c>
-      <c r="F26" s="5">
-        <v>85000</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>131</v>
       </c>
-      <c r="H26" t="s">
-        <v>94</v>
-      </c>
       <c r="I26" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="J26" t="s">
         <v>6</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L26" t="s">
@@ -1998,7 +2074,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>134</v>
       </c>
@@ -2009,36 +2085,36 @@
         <v>2</v>
       </c>
       <c r="E27" s="1">
-        <v>44182</v>
-      </c>
-      <c r="F27" s="5">
-        <v>70000</v>
+        <v>44475</v>
+      </c>
+      <c r="F27" t="s">
+        <v>135</v>
       </c>
       <c r="G27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H27" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="I27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J27" t="s">
-        <v>6</v>
-      </c>
-      <c r="K27" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="L27" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="M27" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" ht="409.6" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -2047,36 +2123,36 @@
         <v>2</v>
       </c>
       <c r="E28" s="1">
-        <v>44180</v>
-      </c>
-      <c r="F28" s="5">
-        <v>450000</v>
+        <v>44446</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1400</v>
       </c>
       <c r="G28" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H28" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="I28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J28" t="s">
-        <v>142</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>143</v>
+        <v>121</v>
+      </c>
+      <c r="K28" t="s">
+        <v>144</v>
       </c>
       <c r="L28" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="M28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -2085,24 +2161,24 @@
         <v>2</v>
       </c>
       <c r="E29" s="1">
-        <v>44061</v>
-      </c>
-      <c r="F29" s="5">
-        <v>65000</v>
+        <v>44441</v>
+      </c>
+      <c r="F29" s="2">
+        <v>225000000</v>
       </c>
       <c r="G29" t="s">
-        <v>146</v>
+        <v>81</v>
       </c>
       <c r="H29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I29" t="s">
         <v>147</v>
       </c>
       <c r="J29" t="s">
-        <v>6</v>
-      </c>
-      <c r="K29" t="s">
+        <v>138</v>
+      </c>
+      <c r="K29" s="3" t="s">
         <v>148</v>
       </c>
       <c r="L29" t="s">
@@ -2112,7 +2188,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>150</v>
       </c>
@@ -2123,69 +2199,259 @@
         <v>2</v>
       </c>
       <c r="E30" s="1">
+        <v>44278</v>
+      </c>
+      <c r="F30" s="2">
+        <v>90000</v>
+      </c>
+      <c r="G30" t="s">
+        <v>151</v>
+      </c>
+      <c r="H30" t="s">
+        <v>65</v>
+      </c>
+      <c r="I30" t="s">
+        <v>152</v>
+      </c>
+      <c r="J30" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30" t="s">
+        <v>153</v>
+      </c>
+      <c r="L30" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>44055</v>
+      </c>
+      <c r="F31" s="2">
+        <v>85000</v>
+      </c>
+      <c r="G31" t="s">
+        <v>156</v>
+      </c>
+      <c r="H31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" t="s">
+        <v>72</v>
+      </c>
+      <c r="J31" t="s">
+        <v>6</v>
+      </c>
+      <c r="K31" t="s">
+        <v>157</v>
+      </c>
+      <c r="L31" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>159</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>44182</v>
+      </c>
+      <c r="F32" s="2">
+        <v>70000</v>
+      </c>
+      <c r="G32" t="s">
+        <v>160</v>
+      </c>
+      <c r="H32" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" t="s">
+        <v>161</v>
+      </c>
+      <c r="J32" t="s">
+        <v>6</v>
+      </c>
+      <c r="K32" t="s">
+        <v>162</v>
+      </c>
+      <c r="L32" t="s">
+        <v>20</v>
+      </c>
+      <c r="M32" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1">
+        <v>44180</v>
+      </c>
+      <c r="F33" s="2">
+        <v>450000</v>
+      </c>
+      <c r="G33" t="s">
+        <v>165</v>
+      </c>
+      <c r="H33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" t="s">
+        <v>166</v>
+      </c>
+      <c r="J33" t="s">
+        <v>167</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L33" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>170</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="1">
+        <v>44061</v>
+      </c>
+      <c r="F34" s="2">
+        <v>65000</v>
+      </c>
+      <c r="G34" t="s">
+        <v>171</v>
+      </c>
+      <c r="H34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I34" t="s">
+        <v>172</v>
+      </c>
+      <c r="J34" t="s">
+        <v>6</v>
+      </c>
+      <c r="K34" t="s">
+        <v>173</v>
+      </c>
+      <c r="L34" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>175</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1">
         <v>44012</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F35" s="2">
         <v>40000</v>
       </c>
-      <c r="G30" t="s">
-        <v>131</v>
-      </c>
-      <c r="H30" t="s">
-        <v>94</v>
-      </c>
-      <c r="I30" t="s">
-        <v>151</v>
-      </c>
-      <c r="J30" t="s">
-        <v>142</v>
-      </c>
-      <c r="K30" t="s">
-        <v>152</v>
-      </c>
-      <c r="L30" t="s">
-        <v>8</v>
-      </c>
-      <c r="M30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>154</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="G35" t="s">
+        <v>156</v>
+      </c>
+      <c r="H35" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" t="s">
+        <v>176</v>
+      </c>
+      <c r="J35" t="s">
+        <v>167</v>
+      </c>
+      <c r="K35" t="s">
+        <v>177</v>
+      </c>
+      <c r="L35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1">
         <v>43968</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F36" s="2">
         <v>75000</v>
       </c>
-      <c r="G31" t="s">
-        <v>131</v>
-      </c>
-      <c r="H31" t="s">
-        <v>94</v>
-      </c>
-      <c r="I31" t="s">
-        <v>155</v>
-      </c>
-      <c r="J31" t="s">
-        <v>13</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="G36" t="s">
         <v>156</v>
       </c>
-      <c r="L31" t="s">
-        <v>8</v>
-      </c>
-      <c r="M31" t="s">
-        <v>157</v>
+      <c r="H36" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" t="s">
+        <v>180</v>
+      </c>
+      <c r="J36" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" t="s">
+        <v>181</v>
+      </c>
+      <c r="L36" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>